<commit_message>
Importação dos Dados Processados pelo Código
</commit_message>
<xml_diff>
--- a/data/processed/coeficientes_rfr.xlsx
+++ b/data/processed/coeficientes_rfr.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A45"/>
+  <dimension ref="A1:B45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,227 +434,454 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="n">
-        <v>0</v>
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>variavel</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>impacto</t>
+        </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>sem instrução ou fundamental incompleto</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
         <v>0.1155507785649469</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>proporção de pessoas com acesso simultâneo aos três serviços de saneamento básico(%)</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
         <v>0.08605211848283119</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>ensino fundamental completo ou médio incompleto</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
         <v>0.07835067026082183</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>rendimento-hora médio real habitual do trabalho principal(r$/hora)</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
         <v>0.07706381732261652</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>rendimento médio real habitual de todos os trabalhos(r$/mês)</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
         <v>0.07248042419352443</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="n">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>rendimento médio real habitual do trabalho principal(r$/mês)</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
         <v>0.06026901336760861</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="n">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>número de beneficiários de plano de saúde</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
         <v>0.05927591338838799</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="n">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>taxa de analfabetismo</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
         <v>0.05308365959162289</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="n">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>ensino superior completo</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
         <v>0.04979966732049831</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="n">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>domicílio cedido por empregador</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
         <v>0.04675801818767016</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="n">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>ensino médio completo ou superior incompleto</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
         <v>0.04380465574193756</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="n">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>outra forma</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
         <v>0.04062919005884222</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="n">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>taxa de formalização</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
         <v>0.03935542976275665</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="n">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>rendimento-hora médio real habitual de todos os trabalhos(r$/hora)</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
         <v>0.03665173174559237</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="n">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>índice gini</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
         <v>0.0305714320890455</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="n">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>população desocupada</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
         <v>0.01151993434358454</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="n">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>nível de ocupação</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
         <v>0.01103289705656737</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="n">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>população subutilizada</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
         <v>0.008292140892715785</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="n">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>taxa total mortalidade</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
         <v>0.008091261555958752</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="n">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>total pessoas ocupadas(1 000 pessoas)</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
         <v>0.00729589095242424</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" t="n">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>70 anos ou mais</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
         <v>0.006739664557998235</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" t="n">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>domicílio alugado</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
         <v>0.005435355703073468</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" t="n">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>domicílio cedido de outra forma</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
         <v>0.00518749975111763</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" t="n">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>taxa de desocupação</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
         <v>0.004747721980339061</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" t="n">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>45 a 59 anos</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
         <v>0.004648301516484312</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" t="n">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>taxa composta de subutilização</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
         <v>0.004497573864427557</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" t="n">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>população na força de trabalho potencial</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
         <v>0.003986587857572095</v>
       </c>
     </row>
     <row r="29">
-      <c r="A29" t="n">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>domicílio próprio - já pago</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
         <v>0.003696777110184935</v>
       </c>
     </row>
     <row r="30">
-      <c r="A30" t="n">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>60 a 69 anos</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
         <v>0.003308591129582522</v>
       </c>
     </row>
     <row r="31">
-      <c r="A31" t="n">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>60 anos ou mais</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
         <v>0.003031108529541404</v>
       </c>
     </row>
     <row r="32">
-      <c r="A32" t="n">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>domicílio cedido por familiar</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
         <v>0.002821688572171627</v>
       </c>
     </row>
     <row r="33">
-      <c r="A33" t="n">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>população ocupada</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
         <v>0.002034654169014393</v>
       </c>
     </row>
     <row r="34">
-      <c r="A34" t="n">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>15 a 29 anos</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
         <v>0.001978161481057872</v>
       </c>
     </row>
     <row r="35">
-      <c r="A35" t="n">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>domicílio próprio - pagando</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
         <v>0.001841626028367157</v>
       </c>
     </row>
     <row r="36">
-      <c r="A36" t="n">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>taxa de participação</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
         <v>0.001797980067057097</v>
       </c>
     </row>
     <row r="37">
-      <c r="A37" t="n">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>número mensal médio de leitos de internação (total)</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
         <v>0.001569957500728899</v>
       </c>
     </row>
     <row r="38">
-      <c r="A38" t="n">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>0 a 14 anos</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
         <v>0.001502197381589015</v>
       </c>
     </row>
     <row r="39">
-      <c r="A39" t="n">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>população ocupada em trabalhos formais</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
         <v>0.001209856861836832</v>
       </c>
     </row>
     <row r="40">
-      <c r="A40" t="n">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>saneamento basico total(1 000 pessoas)</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
         <v>0.001086158994192984</v>
       </c>
     </row>
     <row r="41">
-      <c r="A41" t="n">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>população</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
         <v>0.000951001603266047</v>
       </c>
     </row>
     <row r="42">
-      <c r="A42" t="n">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>população na força de trabalho</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
         <v>0.0006984836478971099</v>
       </c>
     </row>
     <row r="43">
-      <c r="A43" t="n">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>total pessoas por condição de ocupação a domicílio(1 000 pessoas)</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
         <v>0.0005984499261882677</v>
       </c>
     </row>
     <row r="44">
-      <c r="A44" t="n">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>população em idade de trabalhar</t>
+        </is>
+      </c>
+      <c r="B44" t="n">
         <v>0.0005628104162204548</v>
       </c>
     </row>
     <row r="45">
-      <c r="A45" t="n">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>30 a 44 anos</t>
+        </is>
+      </c>
+      <c r="B45" t="n">
         <v>0.0001391464701373478</v>
       </c>
     </row>

</xml_diff>